<commit_message>
se agregaron las colecciones
</commit_message>
<xml_diff>
--- a/configs/Reportes/Companies_Report.xlsx
+++ b/configs/Reportes/Companies_Report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -49,7 +49,13 @@
     <t>prueba d</t>
   </si>
   <si>
-    <t/>
+    <t>programacion</t>
+  </si>
+  <si>
+    <t>impacto al cliente</t>
+  </si>
+  <si>
+    <t>grande empresa</t>
   </si>
   <si>
     <t>c</t>
@@ -61,7 +67,16 @@
     <t>d</t>
   </si>
   <si>
-    <t>grande empresa</t>
+    <t>e</t>
+  </si>
+  <si>
+    <t>pequeña empresa</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>Usuario2</t>
   </si>
 </sst>
 </file>
@@ -133,7 +148,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -195,13 +210,13 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
@@ -209,7 +224,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -221,7 +236,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
@@ -229,7 +244,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
@@ -241,10 +256,50 @@
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>